<commit_message>
Cleaned up data, Added more pivot tables
</commit_message>
<xml_diff>
--- a/results_charted.xlsx
+++ b/results_charted.xlsx
@@ -9,22 +9,23 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Raw Data" sheetId="1" r:id="rId1"/>
     <sheet name="Sex" sheetId="9" r:id="rId2"/>
     <sheet name="Respondents per Member" sheetId="11" r:id="rId3"/>
+    <sheet name="Year Level" sheetId="12" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="8" r:id="rId4"/>
+    <pivotCache cacheId="31" r:id="rId5"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="947" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="975" uniqueCount="94">
   <si>
     <t>Timestamp</t>
   </si>
@@ -152,16 +153,7 @@
     <t>2016/09/15 8:00:55 PM GMT+8</t>
   </si>
   <si>
-    <t>4th - 5th Year</t>
-  </si>
-  <si>
     <t>2016/09/15 8:11:31 PM GMT+8</t>
-  </si>
-  <si>
-    <t>Engineering</t>
-  </si>
-  <si>
-    <t>Lois Velasco</t>
   </si>
   <si>
     <t>2016/09/15 8:59:39 PM GMT+8</t>
@@ -183,9 +175,6 @@
   </si>
   <si>
     <t>2016/09/18 1:58:04 AM GMT+8</t>
-  </si>
-  <si>
-    <t>ENGG</t>
   </si>
   <si>
     <t>Android</t>
@@ -227,9 +216,6 @@
     <t>2016/09/19 7:34:23 PM GMT+8</t>
   </si>
   <si>
-    <t xml:space="preserve"> College of Engineering</t>
-  </si>
-  <si>
     <t>2016/09/19 7:47:50 PM GMT+8</t>
   </si>
   <si>
@@ -248,9 +234,6 @@
     <t>2016/09/19 8:09:26 PM GMT+8</t>
   </si>
   <si>
-    <t>Engg</t>
-  </si>
-  <si>
     <t>2016/09/19 8:22:21 PM GMT+8</t>
   </si>
   <si>
@@ -266,9 +249,6 @@
     <t>2016/09/19 11:38:42 PM GMT+8</t>
   </si>
   <si>
-    <t>CSSP</t>
-  </si>
-  <si>
     <t>2016/09/20 12:03:39 AM GMT+8</t>
   </si>
   <si>
@@ -278,9 +258,6 @@
     <t>2016/09/20 8:51:25 AM GMT+8</t>
   </si>
   <si>
-    <t>CS</t>
-  </si>
-  <si>
     <t>2016/09/20 9:10:46 AM GMT+8</t>
   </si>
   <si>
@@ -288,9 +265,6 @@
   </si>
   <si>
     <t>2016/09/20 10:53:07 PM GMT+8</t>
-  </si>
-  <si>
-    <t>Sabrina Follosco</t>
   </si>
   <si>
     <t>2016/09/21 12:16:20 AM GMT+8</t>
@@ -311,16 +285,28 @@
     <t>College of Human Kinetics</t>
   </si>
   <si>
-    <t>(CAL)College of Arts &amp; Letters</t>
-  </si>
-  <si>
     <t>6th Year</t>
   </si>
   <si>
-    <t>(CSSP)College of Social Sciences &amp; Philosophy</t>
+    <t>Virata School of Business</t>
   </si>
   <si>
-    <t>Virata School of Business</t>
+    <t>Count of Year Level</t>
+  </si>
+  <si>
+    <t>(blank)</t>
+  </si>
+  <si>
+    <t>4th Year</t>
+  </si>
+  <si>
+    <t>5th Year</t>
+  </si>
+  <si>
+    <t>College of Arts and Letters</t>
+  </si>
+  <si>
+    <t>College of Social Science and Philosophy</t>
   </si>
 </sst>
 </file>
@@ -804,7 +790,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
@@ -812,6 +798,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1094,6 +1081,74 @@
           </a:sp3d>
         </c:spPr>
       </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="5"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+          <a:scene3d>
+            <a:camera prst="orthographicFront"/>
+            <a:lightRig rig="brightRoom" dir="t"/>
+          </a:scene3d>
+          <a:sp3d prstMaterial="flat">
+            <a:bevelT w="50800" h="101600" prst="angle"/>
+            <a:contourClr>
+              <a:srgbClr val="000000"/>
+            </a:contourClr>
+          </a:sp3d>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:layout/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:dLblPos val="inEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:separator>. </c:separator>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+              <c15:layout/>
+            </c:ext>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
     </c:pivotFmts>
     <c:plotArea>
       <c:layout/>
@@ -1171,32 +1226,22 @@
           </c:dPt>
           <c:dLbls>
             <c:spPr>
-              <a:solidFill>
-                <a:sysClr val="window" lastClr="FFFFFF"/>
-              </a:solidFill>
+              <a:noFill/>
               <a:ln>
-                <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000">
-                    <a:lumMod val="25000"/>
-                    <a:lumOff val="75000"/>
-                  </a:sysClr>
-                </a:solidFill>
+                <a:noFill/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
                 <a:spAutoFit/>
               </a:bodyPr>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="dk1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
+                      <a:schemeClr val="lt1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -1206,13 +1251,14 @@
                 <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
-            <c:dLblPos val="outEnd"/>
+            <c:dLblPos val="inEnd"/>
             <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="1"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
             <c:showSerName val="0"/>
-            <c:showPercent val="1"/>
+            <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
+            <c:separator>. </c:separator>
             <c:showLeaderLines val="1"/>
             <c:leaderLines>
               <c:spPr>
@@ -1230,15 +1276,6 @@
             </c:leaderLines>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-                  <a:prstGeom prst="wedgeRectCallout">
-                    <a:avLst/>
-                  </a:prstGeom>
-                  <a:noFill/>
-                  <a:ln>
-                    <a:noFill/>
-                  </a:ln>
-                </c15:spPr>
                 <c15:layout/>
               </c:ext>
             </c:extLst>
@@ -1279,8 +1316,9 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="bestFit"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -1565,9 +1603,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Respondents per Member'!$A$4:$A$9</c:f>
+              <c:f>'Respondents per Member'!$A$4:$A$7</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>Carisse Dacuba</c:v>
                 </c:pt>
@@ -1575,15 +1613,9 @@
                   <c:v>Gerard Arel H. Latoga</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Lois Velasco</c:v>
+                  <c:v>Troi Lobaton</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Sabrina Follosco</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Troi Lobaton</c:v>
-                </c:pt>
-                <c:pt idx="5">
                   <c:v>Vincent Paul Fiestada</c:v>
                 </c:pt>
               </c:strCache>
@@ -1591,10 +1623,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Respondents per Member'!$B$4:$B$9</c:f>
+              <c:f>'Respondents per Member'!$B$4:$B$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>12</c:v>
                 </c:pt>
@@ -1602,15 +1634,9 @@
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="5">
                   <c:v>22</c:v>
                 </c:pt>
               </c:numCache>
@@ -1801,6 +1827,446 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:pivotSource>
+    <c:name>[results_charted.xlsx]Year Level!PivotTable3</c:name>
+    <c:fmtId val="0"/>
+  </c:pivotSource>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="20" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-PH"/>
+              <a:t>Count of Year Level</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="20" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Year Level'!$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="110000"/>
+                    <a:satMod val="105000"/>
+                    <a:tint val="67000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="105000"/>
+                    <a:satMod val="103000"/>
+                    <a:tint val="73000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="105000"/>
+                    <a:satMod val="109000"/>
+                    <a:tint val="81000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:shade val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>'Year Level'!$A$4:$B$16</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="13"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>College of Fine Arts</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>College of Engineering</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>College of Science</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Virata School of Business</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>College of Engineering</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>College of Human Kinetics</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>College of Social Science and Philosophy</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>College of Arts and Letters</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>(blank)</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>College of Engineering</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>College of Science</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>College of Social Science and Philosophy</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>College of Engineering</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>1st Year</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>2nd Year</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>3rd Year</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>6th Year</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>(blank)</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>4th Year</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>5th Year</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Year Level'!$C$4:$C$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D72E-4B80-9D5B-4DA0E75038B4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="100"/>
+        <c:axId val="558315072"/>
+        <c:axId val="558311328"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="558315072"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="558311328"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="558311328"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="558315072"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst>
+    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
+      <c14:pivotOptions>
+        <c14:dropZoneFilter val="1"/>
+        <c14:dropZoneCategories val="1"/>
+        <c14:dropZoneData val="1"/>
+        <c14:dropZonesVisible val="1"/>
+      </c14:pivotOptions>
+    </c:ext>
+    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{E28EC0CA-F0BB-4C9C-879D-F8772B89E7AC}">
+      <c16:pivotOptions16>
+        <c16:showExpandCollapseFieldButtons val="1"/>
+      </c16:pivotOptions16>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1842,6 +2308,46 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -2923,6 +3429,531 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="219">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="2">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="1"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:shade val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="2">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="1"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:shade val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="2">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="1"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="15875" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="2">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="1"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:shade val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="4"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="2"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" kern="1200" cap="none" spc="20" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="2"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -2993,23 +4024,83 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>266699</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>57149</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>104774</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>81643</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Vincent Paul Fiestada" refreshedDate="42634.8440275463" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="46">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Vincent Paul Fiestada" refreshedDate="42634.876256828706" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="46">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:U47" sheet="Raw Data"/>
   </cacheSource>
   <cacheFields count="21">
     <cacheField name="Timestamp" numFmtId="0">
-      <sharedItems containsDate="1" containsBlank="1" containsMixedTypes="1" minDate="2016-09-20T00:00:00" maxDate="2016-09-21T00:00:00"/>
+      <sharedItems containsDate="1" containsMixedTypes="1" minDate="2016-09-20T00:00:00" maxDate="2016-09-21T00:00:00"/>
     </cacheField>
     <cacheField name="Student Number" numFmtId="0">
       <sharedItems containsMixedTypes="1" containsNumber="1" containsInteger="1" minValue="20131526" maxValue="201689078"/>
     </cacheField>
     <cacheField name="College" numFmtId="0">
-      <sharedItems containsBlank="1"/>
+      <sharedItems containsBlank="1" count="15">
+        <m/>
+        <s v="College of Engineering"/>
+        <s v="College of Science"/>
+        <s v="College of Social Science and Philosophy"/>
+        <s v="College of Fine Arts"/>
+        <s v="College of Human Kinetics"/>
+        <s v="College of Arts and Letters"/>
+        <s v="Virata School of Business"/>
+        <s v="(CSSP)College of Social Sciences &amp; Philosophy" u="1"/>
+        <s v="CSSP" u="1"/>
+        <s v=" College of Engineering" u="1"/>
+        <s v="Engineering" u="1"/>
+        <s v="CS" u="1"/>
+        <s v="(CAL)College of Arts &amp; Letters" u="1"/>
+        <s v="ENGG" u="1"/>
+      </sharedItems>
     </cacheField>
     <cacheField name="Year Level" numFmtId="0">
-      <sharedItems containsBlank="1"/>
+      <sharedItems containsBlank="1" count="8">
+        <m/>
+        <s v="4th Year"/>
+        <s v="2nd Year"/>
+        <s v="3rd Year"/>
+        <s v="5th Year"/>
+        <s v="1st Year"/>
+        <s v="6th Year"/>
+        <s v="4th - 5th Year" u="1"/>
+      </sharedItems>
     </cacheField>
     <cacheField name="Sex" numFmtId="0">
       <sharedItems count="2">
@@ -3022,9 +4113,9 @@
         <s v="Gerard Arel H. Latoga"/>
         <s v="Vincent Paul Fiestada"/>
         <s v="Troi Lobaton"/>
-        <s v="Lois Velasco"/>
         <s v="Carisse Dacuba"/>
-        <s v="Sabrina Follosco"/>
+        <s v="Sabrina Follosco" u="1"/>
+        <s v="Lois Velasco" u="1"/>
       </sharedItems>
     </cacheField>
     <cacheField name="Which of these products are you familiar with?" numFmtId="0">
@@ -3086,8 +4177,8 @@
   <r>
     <s v="2016/09/13 10:50:44 PM GMT+8"/>
     <s v="Carina Tesoro"/>
-    <m/>
-    <m/>
+    <x v="0"/>
+    <x v="0"/>
     <x v="0"/>
     <x v="0"/>
     <s v="iPhones &amp; iPads;Galaxy Phones &amp; Tablets;Android"/>
@@ -3109,8 +4200,8 @@
   <r>
     <s v="2016/09/13 10:50:45 PM GMT+8"/>
     <s v="Faith Therese F. Pena"/>
-    <m/>
-    <s v="4th - 5th Year"/>
+    <x v="1"/>
+    <x v="1"/>
     <x v="0"/>
     <x v="0"/>
     <s v="iPhones &amp; iPads;Galaxy Phones &amp; Tablets;Java;Android"/>
@@ -3132,8 +4223,8 @@
   <r>
     <s v="2016/09/14 10:59:42 PM GMT+8"/>
     <n v="201502372"/>
-    <s v="College of Science"/>
-    <s v="2nd Year"/>
+    <x v="2"/>
+    <x v="2"/>
     <x v="0"/>
     <x v="1"/>
     <s v="iPhones &amp; iPads;Galaxy Phones &amp; Tablets;Java;Android"/>
@@ -3155,8 +4246,8 @@
   <r>
     <s v="2016/09/15 6:14:40 PM GMT+8"/>
     <n v="201513612"/>
-    <s v="College of Engineering"/>
-    <s v="2nd Year"/>
+    <x v="1"/>
+    <x v="2"/>
     <x v="1"/>
     <x v="2"/>
     <s v="iPhones &amp; iPads;Galaxy Phones &amp; Tablets;Android"/>
@@ -3178,8 +4269,8 @@
   <r>
     <s v="2016/09/15 7:49:34 PM GMT+8"/>
     <n v="201451498"/>
-    <s v="College of Engineering"/>
-    <s v="3rd Year"/>
+    <x v="1"/>
+    <x v="3"/>
     <x v="0"/>
     <x v="2"/>
     <s v="iPhones &amp; iPads;Galaxy Phones &amp; Tablets;Java;Android"/>
@@ -3201,8 +4292,8 @@
   <r>
     <s v="2016/09/15 8:00:55 PM GMT+8"/>
     <n v="201301872"/>
-    <s v="College of Science"/>
-    <s v="4th - 5th Year"/>
+    <x v="2"/>
+    <x v="1"/>
     <x v="0"/>
     <x v="2"/>
     <s v="iPhones &amp; iPads;Galaxy Phones &amp; Tablets;Android"/>
@@ -3224,10 +4315,10 @@
   <r>
     <s v="2016/09/15 8:11:31 PM GMT+8"/>
     <n v="201454693"/>
-    <s v="Engineering"/>
-    <s v="3rd Year"/>
     <x v="1"/>
     <x v="3"/>
+    <x v="1"/>
+    <x v="2"/>
     <s v="iPhones &amp; iPads;Galaxy Phones &amp; Tablets;Java;Android"/>
     <s v="Yes"/>
     <s v="No"/>
@@ -3247,8 +4338,8 @@
   <r>
     <s v="2016/09/15 8:59:39 PM GMT+8"/>
     <n v="201314723"/>
-    <s v="College of Science"/>
-    <s v="4th - 5th Year"/>
+    <x v="2"/>
+    <x v="1"/>
     <x v="0"/>
     <x v="2"/>
     <s v="iPhones &amp; iPads;Galaxy Phones &amp; Tablets;Java;Android"/>
@@ -3270,10 +4361,10 @@
   <r>
     <s v="2016/09/18 1:21:27 AM GMT+8"/>
     <n v="201130511"/>
-    <s v="College of Engineering"/>
-    <s v="4th - 5th Year"/>
     <x v="1"/>
     <x v="4"/>
+    <x v="1"/>
+    <x v="3"/>
     <s v="iPhones &amp; iPads;Galaxy Phones &amp; Tablets;Android"/>
     <s v="No"/>
     <s v="No"/>
@@ -3293,10 +4384,10 @@
   <r>
     <s v="2016/09/18 1:26:53 AM GMT+8"/>
     <n v="201466214"/>
-    <s v="College of Engineering"/>
-    <s v="3rd Year"/>
+    <x v="1"/>
+    <x v="3"/>
     <x v="0"/>
-    <x v="4"/>
+    <x v="3"/>
     <s v="iPhones &amp; iPads"/>
     <s v="No"/>
     <s v="No"/>
@@ -3316,10 +4407,10 @@
   <r>
     <s v="2016/09/18 1:58:04 AM GMT+8"/>
     <n v="201378766"/>
-    <s v="ENGG"/>
-    <s v="4th - 5th Year"/>
     <x v="1"/>
-    <x v="4"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="3"/>
     <s v="Android"/>
     <s v="No"/>
     <s v="No"/>
@@ -3339,10 +4430,10 @@
   <r>
     <s v="2016/09/18 9:11:17 AM GMT+8"/>
     <n v="201101515"/>
-    <s v="College of Engineering"/>
-    <s v="4th - 5th Year"/>
+    <x v="1"/>
+    <x v="4"/>
     <x v="0"/>
-    <x v="4"/>
+    <x v="3"/>
     <s v="iPhones &amp; iPads;Galaxy Phones &amp; Tablets;Java;Android"/>
     <s v="Yes"/>
     <s v="No"/>
@@ -3362,10 +4453,10 @@
   <r>
     <s v="2016/09/18 10:10:07 AM GMT+8"/>
     <n v="201313012"/>
-    <s v="College of Engineering"/>
-    <s v="4th - 5th Year"/>
+    <x v="1"/>
+    <x v="1"/>
     <x v="0"/>
-    <x v="4"/>
+    <x v="3"/>
     <s v="iPhones &amp; iPads;Galaxy Phones &amp; Tablets;Android"/>
     <s v="Yes"/>
     <s v="No"/>
@@ -3385,10 +4476,10 @@
   <r>
     <s v="2016/09/18 11:38:17 AM GMT+8"/>
     <n v="201359474"/>
-    <s v="College of Engineering"/>
-    <s v="4th - 5th Year"/>
     <x v="1"/>
-    <x v="4"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="3"/>
     <s v="iPhones &amp; iPads;Galaxy Phones &amp; Tablets;Java;Android"/>
     <s v="No"/>
     <s v="No"/>
@@ -3408,10 +4499,10 @@
   <r>
     <s v="2016/09/18 2:49:17 PM GMT+8"/>
     <n v="201116701"/>
-    <s v="College of Engineering"/>
-    <s v="4th - 5th Year"/>
+    <x v="1"/>
+    <x v="4"/>
     <x v="0"/>
-    <x v="4"/>
+    <x v="3"/>
     <s v="iPhones &amp; iPads;Galaxy Phones &amp; Tablets;Java;Android"/>
     <s v="Yes"/>
     <s v="Yes"/>
@@ -3431,10 +4522,10 @@
   <r>
     <s v="2016/09/18 7:50:21 PM GMT+8"/>
     <n v="201259002"/>
-    <s v="College of Engineering"/>
-    <s v="4th - 5th Year"/>
+    <x v="1"/>
+    <x v="4"/>
     <x v="0"/>
-    <x v="4"/>
+    <x v="3"/>
     <s v="iPhones &amp; iPads;Galaxy Phones &amp; Tablets;Java;Android"/>
     <s v="Yes"/>
     <s v="Yes"/>
@@ -3454,8 +4545,8 @@
   <r>
     <s v="2016/09/18 9:38:54 PM GMT+8"/>
     <n v="201314726"/>
-    <s v="College of Engineering"/>
-    <s v="4th - 5th Year"/>
+    <x v="1"/>
+    <x v="1"/>
     <x v="1"/>
     <x v="0"/>
     <s v="iPhones &amp; iPads"/>
@@ -3477,8 +4568,8 @@
   <r>
     <s v="2016/09/18 10:31:23 PM GMT+8"/>
     <n v="201314815"/>
-    <s v="College of Engineering"/>
-    <s v="4th - 5th Year"/>
+    <x v="1"/>
+    <x v="1"/>
     <x v="1"/>
     <x v="0"/>
     <s v="Android"/>
@@ -3500,10 +4591,10 @@
   <r>
     <s v="2016/09/19 6:15:48 PM GMT+8"/>
     <n v="201301809"/>
-    <s v="College of Engineering"/>
-    <s v="4th - 5th Year"/>
+    <x v="1"/>
+    <x v="1"/>
     <x v="0"/>
-    <x v="4"/>
+    <x v="3"/>
     <s v="iPhones &amp; iPads;Android"/>
     <s v="Yes"/>
     <s v="Yes"/>
@@ -3523,8 +4614,8 @@
   <r>
     <s v="2016/09/19 7:33:21 PM GMT+8"/>
     <n v="201358103"/>
-    <s v="Engineering"/>
-    <s v="4th - 5th Year"/>
+    <x v="1"/>
+    <x v="1"/>
     <x v="1"/>
     <x v="1"/>
     <s v="iPhones &amp; iPads;Galaxy Phones &amp; Tablets;Java;Android"/>
@@ -3546,8 +4637,8 @@
   <r>
     <s v="2016/09/19 7:34:23 PM GMT+8"/>
     <n v="201262449"/>
-    <s v=" College of Engineering"/>
-    <s v="4th - 5th Year"/>
+    <x v="1"/>
+    <x v="4"/>
     <x v="1"/>
     <x v="1"/>
     <s v="iPhones &amp; iPads;Galaxy Phones &amp; Tablets;Java;Android"/>
@@ -3569,8 +4660,8 @@
   <r>
     <s v="2016/09/19 7:47:50 PM GMT+8"/>
     <n v="201300167"/>
-    <s v="College of Engineering"/>
-    <s v="4th - 5th Year"/>
+    <x v="1"/>
+    <x v="1"/>
     <x v="1"/>
     <x v="1"/>
     <s v="iPhones &amp; iPads;Galaxy Phones &amp; Tablets"/>
@@ -3592,8 +4683,8 @@
   <r>
     <s v="2016/09/19 7:53:39 PM GMT+8"/>
     <n v="201260357"/>
-    <s v="College of Engineering"/>
-    <s v="4th - 5th Year"/>
+    <x v="1"/>
+    <x v="4"/>
     <x v="0"/>
     <x v="1"/>
     <s v="iPhones &amp; iPads;Galaxy Phones &amp; Tablets;Java;Android"/>
@@ -3615,8 +4706,8 @@
   <r>
     <s v="2016/09/19 8:05:36 PM GMT+8"/>
     <n v="201162632"/>
-    <s v="College of Engineering"/>
-    <s v="4th - 5th Year"/>
+    <x v="1"/>
+    <x v="4"/>
     <x v="0"/>
     <x v="1"/>
     <s v="iPhones &amp; iPads;Java;Android"/>
@@ -3638,8 +4729,8 @@
   <r>
     <s v="2016/09/19 8:09:26 PM GMT+8"/>
     <n v="201523456"/>
-    <s v="ENGG"/>
-    <s v="4th - 5th Year"/>
+    <x v="1"/>
+    <x v="4"/>
     <x v="1"/>
     <x v="1"/>
     <s v="iPhones &amp; iPads;Galaxy Phones &amp; Tablets;Java;Android"/>
@@ -3661,8 +4752,8 @@
   <r>
     <s v="2016/09/19 8:22:21 PM GMT+8"/>
     <n v="201310167"/>
-    <s v="College of Engineering"/>
-    <s v="4th - 5th Year"/>
+    <x v="1"/>
+    <x v="1"/>
     <x v="1"/>
     <x v="1"/>
     <s v="iPhones &amp; iPads;Galaxy Phones &amp; Tablets;Java;Android"/>
@@ -3684,8 +4775,8 @@
   <r>
     <s v="2016/09/19 8:56:08 PM GMT+8"/>
     <n v="201304448"/>
-    <s v="College of Engineering"/>
-    <s v="4th - 5th Year"/>
+    <x v="1"/>
+    <x v="1"/>
     <x v="1"/>
     <x v="1"/>
     <s v="iPhones &amp; iPads;Galaxy Phones &amp; Tablets;Android"/>
@@ -3707,8 +4798,8 @@
   <r>
     <s v="2016/09/19 9:23:53 PM GMT+8"/>
     <n v="200664076"/>
-    <s v="College of Engineering"/>
-    <s v="3rd Year"/>
+    <x v="1"/>
+    <x v="3"/>
     <x v="0"/>
     <x v="1"/>
     <s v="Android"/>
@@ -3730,8 +4821,8 @@
   <r>
     <s v="2016/09/19 9:37:35 PM GMT+8"/>
     <n v="201122222"/>
-    <s v="College of Engineering"/>
-    <s v="4th - 5th Year"/>
+    <x v="1"/>
+    <x v="4"/>
     <x v="1"/>
     <x v="1"/>
     <s v="iPhones &amp; iPads;Galaxy Phones &amp; Tablets;Java;Android"/>
@@ -3753,8 +4844,8 @@
   <r>
     <s v="2016/09/19 11:38:42 PM GMT+8"/>
     <n v="201358229"/>
-    <s v="CSSP"/>
-    <s v="4th - 5th Year"/>
+    <x v="3"/>
+    <x v="1"/>
     <x v="1"/>
     <x v="1"/>
     <s v="iPhones &amp; iPads;Galaxy Phones &amp; Tablets;Java;Android"/>
@@ -3776,10 +4867,10 @@
   <r>
     <s v="2016/09/20 12:03:39 AM GMT+8"/>
     <n v="201328739"/>
-    <s v="College of Engineering"/>
-    <s v="4th - 5th Year"/>
+    <x v="1"/>
+    <x v="1"/>
     <x v="0"/>
-    <x v="4"/>
+    <x v="3"/>
     <s v="iPhones &amp; iPads;Galaxy Phones &amp; Tablets;Java;Android"/>
     <s v="No"/>
     <s v="Yes"/>
@@ -3799,10 +4890,10 @@
   <r>
     <s v="2016/09/20 8:40:50 AM GMT+8"/>
     <n v="201504145"/>
-    <s v="College of Engineering"/>
-    <s v="2nd Year"/>
+    <x v="1"/>
+    <x v="2"/>
     <x v="0"/>
-    <x v="4"/>
+    <x v="3"/>
     <s v="iPhones &amp; iPads;Galaxy Phones &amp; Tablets;Android"/>
     <s v="Yes"/>
     <s v="No"/>
@@ -3822,8 +4913,8 @@
   <r>
     <s v="2016/09/20 8:51:25 AM GMT+8"/>
     <n v="201303453"/>
-    <s v="CS"/>
-    <s v="4th - 5th Year"/>
+    <x v="2"/>
+    <x v="1"/>
     <x v="1"/>
     <x v="1"/>
     <s v="iPhones &amp; iPads;Galaxy Phones &amp; Tablets;Java;Android"/>
@@ -3845,10 +4936,10 @@
   <r>
     <s v="2016/09/20 9:10:46 AM GMT+8"/>
     <n v="201337092"/>
-    <s v="ENGG"/>
-    <s v="4th - 5th Year"/>
     <x v="1"/>
-    <x v="4"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="3"/>
     <s v="iPhones &amp; iPads;Android"/>
     <s v="Yes"/>
     <s v="Yes"/>
@@ -3868,8 +4959,8 @@
   <r>
     <s v="2016/09/20 10:27:13 PM GMT+8"/>
     <n v="20134865"/>
-    <s v="CS"/>
-    <s v="4th - 5th Year"/>
+    <x v="2"/>
+    <x v="1"/>
     <x v="0"/>
     <x v="0"/>
     <s v="iPhones &amp; iPads;Galaxy Phones &amp; Tablets;Android"/>
@@ -3891,10 +4982,10 @@
   <r>
     <s v="2016/09/20 10:53:07 PM GMT+8"/>
     <n v="20131526"/>
-    <s v="College of Engineering"/>
-    <s v="4th - 5th Year"/>
     <x v="1"/>
-    <x v="5"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="2"/>
     <s v="Android"/>
     <s v="No"/>
     <s v="Yes"/>
@@ -3914,8 +5005,8 @@
   <r>
     <s v="2016/09/21 12:16:20 AM GMT+8"/>
     <n v="201314912"/>
-    <s v="ENGG"/>
-    <s v="4th - 5th Year"/>
+    <x v="1"/>
+    <x v="1"/>
     <x v="0"/>
     <x v="0"/>
     <s v="Android"/>
@@ -3937,8 +5028,8 @@
   <r>
     <d v="2016-09-20T00:00:00"/>
     <n v="201689078"/>
-    <s v="College of Fine Arts"/>
-    <s v="1st Year"/>
+    <x v="4"/>
+    <x v="5"/>
     <x v="0"/>
     <x v="1"/>
     <s v="iPhones &amp; iPads;Galaxy Phones &amp; Tablets;Android"/>
@@ -3960,8 +5051,8 @@
   <r>
     <d v="2016-09-20T00:00:00"/>
     <n v="201489146"/>
-    <s v="College of Human Kinetics"/>
-    <s v="3rd Year"/>
+    <x v="5"/>
+    <x v="3"/>
     <x v="1"/>
     <x v="1"/>
     <s v="iPhones &amp; iPads;Galaxy Phones &amp; Tablets;Android"/>
@@ -3983,8 +5074,8 @@
   <r>
     <d v="2016-09-20T00:00:00"/>
     <n v="201152036"/>
-    <s v="(CAL)College of Arts &amp; Letters"/>
-    <s v="6th Year"/>
+    <x v="6"/>
+    <x v="6"/>
     <x v="0"/>
     <x v="1"/>
     <s v="iPhones &amp; iPads;Galaxy Phones &amp; Tablets;Java;Android"/>
@@ -4006,8 +5097,8 @@
   <r>
     <d v="2016-09-20T00:00:00"/>
     <n v="201406760"/>
-    <s v="(CSSP)College of Social Sciences &amp; Philosophy"/>
-    <s v="3rd Year"/>
+    <x v="3"/>
+    <x v="3"/>
     <x v="0"/>
     <x v="1"/>
     <s v="iPhones &amp; iPads;Galaxy Phones &amp; Tablets;Java;Android"/>
@@ -4027,10 +5118,10 @@
     <s v="Just a part of their profits"/>
   </r>
   <r>
-    <m/>
+    <d v="2016-09-20T00:00:00"/>
     <n v="201510694"/>
-    <s v="Virata School of Business"/>
-    <s v="2nd Year"/>
+    <x v="7"/>
+    <x v="2"/>
     <x v="0"/>
     <x v="1"/>
     <s v="iPhones &amp; iPads;Galaxy Phones &amp; Tablets;Android"/>
@@ -4052,8 +5143,8 @@
   <r>
     <d v="2016-09-20T00:00:00"/>
     <n v="201502985"/>
-    <s v="Virata School of Business"/>
-    <s v="2nd Year"/>
+    <x v="7"/>
+    <x v="2"/>
     <x v="0"/>
     <x v="1"/>
     <s v="Android"/>
@@ -4075,8 +5166,8 @@
   <r>
     <d v="2016-09-20T00:00:00"/>
     <n v="201504580"/>
-    <s v="College of Engineering"/>
-    <s v="2nd Year"/>
+    <x v="1"/>
+    <x v="2"/>
     <x v="0"/>
     <x v="1"/>
     <s v="iPhones &amp; iPads;Galaxy Phones &amp; Tablets;Java;Android"/>
@@ -4098,8 +5189,8 @@
   <r>
     <d v="2016-09-20T00:00:00"/>
     <n v="201504560"/>
-    <s v="College of Engineering"/>
-    <s v="2nd Year"/>
+    <x v="1"/>
+    <x v="2"/>
     <x v="0"/>
     <x v="1"/>
     <s v="iPhones &amp; iPads;Galaxy Phones &amp; Tablets;Java;Android"/>
@@ -4121,8 +5212,8 @@
   <r>
     <d v="2016-09-20T00:00:00"/>
     <n v="201502082"/>
-    <s v="College of Science"/>
-    <s v="2nd Year"/>
+    <x v="2"/>
+    <x v="2"/>
     <x v="1"/>
     <x v="1"/>
     <s v="iPhones &amp; iPads;Galaxy Phones &amp; Tablets;Java;Android"/>
@@ -4145,7 +5236,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable21" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable21" cacheId="31" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="1">
   <location ref="A3:B5" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="21">
     <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
@@ -4317,36 +5408,12 @@
   <dataFields count="1">
     <dataField name="Count of Sex" fld="4" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
-  <chartFormats count="3">
-    <chartFormat chart="0" format="2" series="1">
+  <chartFormats count="1">
+    <chartFormat chart="0" format="5" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
             <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="3">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="4" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="4">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="4" count="1" selected="0">
-            <x v="1"/>
           </reference>
         </references>
       </pivotArea>
@@ -4362,8 +5429,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable28" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="1">
-  <location ref="A3:B9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable28" cacheId="31" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="1">
+  <location ref="A3:B7" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="21">
     <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
       <extLst>
@@ -4402,10 +5469,10 @@
     </pivotField>
     <pivotField axis="axisRow" dataField="1" compact="0" outline="0" showAll="0" defaultSubtotal="0">
       <items count="6">
-        <item x="4"/>
+        <item x="3"/>
         <item x="0"/>
-        <item x="3"/>
-        <item x="5"/>
+        <item m="1" x="5"/>
+        <item m="1" x="4"/>
         <item x="2"/>
         <item x="1"/>
       </items>
@@ -4524,18 +5591,12 @@
   <rowFields count="1">
     <field x="5"/>
   </rowFields>
-  <rowItems count="6">
+  <rowItems count="4">
     <i>
       <x/>
     </i>
     <i>
       <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
     </i>
     <i>
       <x v="4"/>
@@ -4552,6 +5613,263 @@
   </dataFields>
   <chartFormats count="1">
     <chartFormat chart="0" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" fillDownLabelsDefault="1" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="31" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="2">
+  <location ref="A3:C16" firstHeaderRow="1" firstDataRow="1" firstDataCol="2"/>
+  <pivotFields count="21">
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <items count="15">
+        <item m="1" x="10"/>
+        <item m="1" x="13"/>
+        <item m="1" x="8"/>
+        <item x="1"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="2"/>
+        <item m="1" x="12"/>
+        <item m="1" x="9"/>
+        <item m="1" x="14"/>
+        <item m="1" x="11"/>
+        <item x="7"/>
+        <item x="0"/>
+        <item x="3"/>
+        <item x="6"/>
+      </items>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField axis="axisRow" dataField="1" compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <items count="8">
+        <item x="5"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item m="1" x="7"/>
+        <item x="6"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="4"/>
+      </items>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="3"/>
+    <field x="2"/>
+  </rowFields>
+  <rowItems count="13">
+    <i>
+      <x/>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="1"/>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
+    <i r="1">
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="2"/>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="4"/>
+      <x v="14"/>
+    </i>
+    <i>
+      <x v="5"/>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="6"/>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
+    <i r="1">
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="7"/>
+      <x v="3"/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Year Level" fld="3" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="1">
+    <chartFormat chart="0" format="2" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -4775,15 +6093,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V52"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+    <sheetView topLeftCell="C28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F52" sqref="F52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.109375" customWidth="1"/>
     <col min="2" max="2" width="21.88671875" customWidth="1"/>
-    <col min="3" max="3" width="14.109375" customWidth="1"/>
+    <col min="3" max="3" width="39.6640625" customWidth="1"/>
     <col min="4" max="4" width="16.21875" customWidth="1"/>
     <col min="6" max="6" width="22.6640625" customWidth="1"/>
     <col min="7" max="7" width="8.88671875" customWidth="1"/>
@@ -4925,8 +6243,11 @@
       <c r="B3" t="s">
         <v>27</v>
       </c>
+      <c r="C3" t="s">
+        <v>36</v>
+      </c>
       <c r="D3" t="s">
-        <v>42</v>
+        <v>90</v>
       </c>
       <c r="E3" t="s">
         <v>33</v>
@@ -5189,7 +6510,7 @@
         <v>31</v>
       </c>
       <c r="D7" t="s">
-        <v>42</v>
+        <v>90</v>
       </c>
       <c r="E7" t="s">
         <v>33</v>
@@ -5245,13 +6566,13 @@
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B8">
         <v>201454693</v>
       </c>
       <c r="C8" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D8" t="s">
         <v>40</v>
@@ -5260,7 +6581,7 @@
         <v>37</v>
       </c>
       <c r="F8" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="G8" t="s">
         <v>29</v>
@@ -5310,7 +6631,7 @@
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B9">
         <v>201314723</v>
@@ -5319,7 +6640,7 @@
         <v>31</v>
       </c>
       <c r="D9" t="s">
-        <v>42</v>
+        <v>90</v>
       </c>
       <c r="E9" t="s">
         <v>33</v>
@@ -5375,7 +6696,7 @@
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B10">
         <v>201130511</v>
@@ -5384,13 +6705,13 @@
         <v>36</v>
       </c>
       <c r="D10" t="s">
-        <v>42</v>
+        <v>91</v>
       </c>
       <c r="E10" t="s">
         <v>37</v>
       </c>
       <c r="F10" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G10" t="s">
         <v>22</v>
@@ -5440,7 +6761,7 @@
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B11">
         <v>201466214</v>
@@ -5455,10 +6776,10 @@
         <v>33</v>
       </c>
       <c r="F11" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G11" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="H11" t="s">
         <v>23</v>
@@ -5500,30 +6821,30 @@
         <v>24</v>
       </c>
       <c r="U11" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B12">
         <v>201378766</v>
       </c>
       <c r="C12" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="D12" t="s">
-        <v>42</v>
+        <v>90</v>
       </c>
       <c r="E12" t="s">
         <v>37</v>
       </c>
       <c r="F12" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G12" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="H12" t="s">
         <v>23</v>
@@ -5570,7 +6891,7 @@
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B13">
         <v>201101515</v>
@@ -5579,13 +6900,13 @@
         <v>36</v>
       </c>
       <c r="D13" t="s">
-        <v>42</v>
+        <v>91</v>
       </c>
       <c r="E13" t="s">
         <v>33</v>
       </c>
       <c r="F13" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G13" t="s">
         <v>29</v>
@@ -5630,12 +6951,12 @@
         <v>24</v>
       </c>
       <c r="U13" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B14">
         <v>201313012</v>
@@ -5644,13 +6965,13 @@
         <v>36</v>
       </c>
       <c r="D14" t="s">
-        <v>42</v>
+        <v>90</v>
       </c>
       <c r="E14" t="s">
         <v>33</v>
       </c>
       <c r="F14" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G14" t="s">
         <v>22</v>
@@ -5700,7 +7021,7 @@
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B15">
         <v>201359474</v>
@@ -5709,13 +7030,13 @@
         <v>36</v>
       </c>
       <c r="D15" t="s">
-        <v>42</v>
+        <v>90</v>
       </c>
       <c r="E15" t="s">
         <v>37</v>
       </c>
       <c r="F15" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G15" t="s">
         <v>29</v>
@@ -5765,7 +7086,7 @@
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B16">
         <v>201116701</v>
@@ -5774,13 +7095,13 @@
         <v>36</v>
       </c>
       <c r="D16" t="s">
-        <v>42</v>
+        <v>91</v>
       </c>
       <c r="E16" t="s">
         <v>33</v>
       </c>
       <c r="F16" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G16" t="s">
         <v>29</v>
@@ -5825,12 +7146,12 @@
         <v>23</v>
       </c>
       <c r="U16" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B17">
         <v>201259002</v>
@@ -5839,13 +7160,13 @@
         <v>36</v>
       </c>
       <c r="D17" t="s">
-        <v>42</v>
+        <v>91</v>
       </c>
       <c r="E17" t="s">
         <v>33</v>
       </c>
       <c r="F17" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G17" t="s">
         <v>29</v>
@@ -5895,7 +7216,7 @@
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B18">
         <v>201314726</v>
@@ -5904,7 +7225,7 @@
         <v>36</v>
       </c>
       <c r="D18" t="s">
-        <v>42</v>
+        <v>90</v>
       </c>
       <c r="E18" t="s">
         <v>37</v>
@@ -5913,7 +7234,7 @@
         <v>28</v>
       </c>
       <c r="G18" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="H18" t="s">
         <v>23</v>
@@ -5960,7 +7281,7 @@
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B19">
         <v>201314815</v>
@@ -5969,7 +7290,7 @@
         <v>36</v>
       </c>
       <c r="D19" t="s">
-        <v>42</v>
+        <v>90</v>
       </c>
       <c r="E19" t="s">
         <v>37</v>
@@ -5978,7 +7299,7 @@
         <v>28</v>
       </c>
       <c r="G19" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="H19" t="s">
         <v>24</v>
@@ -6025,7 +7346,7 @@
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B20">
         <v>201301809</v>
@@ -6034,16 +7355,16 @@
         <v>36</v>
       </c>
       <c r="D20" t="s">
-        <v>42</v>
+        <v>90</v>
       </c>
       <c r="E20" t="s">
         <v>33</v>
       </c>
       <c r="F20" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G20" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="H20" t="s">
         <v>24</v>
@@ -6090,16 +7411,16 @@
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B21">
         <v>201358103</v>
       </c>
       <c r="C21" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D21" t="s">
-        <v>42</v>
+        <v>90</v>
       </c>
       <c r="E21" t="s">
         <v>37</v>
@@ -6155,16 +7476,16 @@
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B22">
         <v>201262449</v>
       </c>
       <c r="C22" t="s">
-        <v>67</v>
+        <v>36</v>
       </c>
       <c r="D22" t="s">
-        <v>42</v>
+        <v>91</v>
       </c>
       <c r="E22" t="s">
         <v>37</v>
@@ -6220,7 +7541,7 @@
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B23">
         <v>201300167</v>
@@ -6229,7 +7550,7 @@
         <v>36</v>
       </c>
       <c r="D23" t="s">
-        <v>42</v>
+        <v>90</v>
       </c>
       <c r="E23" t="s">
         <v>37</v>
@@ -6238,7 +7559,7 @@
         <v>34</v>
       </c>
       <c r="G23" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="H23" t="s">
         <v>24</v>
@@ -6285,7 +7606,7 @@
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B24">
         <v>201260357</v>
@@ -6294,7 +7615,7 @@
         <v>36</v>
       </c>
       <c r="D24" t="s">
-        <v>42</v>
+        <v>91</v>
       </c>
       <c r="E24" t="s">
         <v>33</v>
@@ -6350,7 +7671,7 @@
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B25">
         <v>201162632</v>
@@ -6359,7 +7680,7 @@
         <v>36</v>
       </c>
       <c r="D25" t="s">
-        <v>42</v>
+        <v>91</v>
       </c>
       <c r="E25" t="s">
         <v>33</v>
@@ -6368,7 +7689,7 @@
         <v>34</v>
       </c>
       <c r="G25" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="H25" t="s">
         <v>24</v>
@@ -6415,16 +7736,16 @@
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B26">
         <v>201523456</v>
       </c>
       <c r="C26" t="s">
-        <v>74</v>
-      </c>
-      <c r="D26" t="s">
-        <v>42</v>
+        <v>36</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>91</v>
       </c>
       <c r="E26" t="s">
         <v>37</v>
@@ -6480,7 +7801,7 @@
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B27">
         <v>201310167</v>
@@ -6489,7 +7810,7 @@
         <v>36</v>
       </c>
       <c r="D27" t="s">
-        <v>42</v>
+        <v>90</v>
       </c>
       <c r="E27" t="s">
         <v>37</v>
@@ -6545,7 +7866,7 @@
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B28">
         <v>201304448</v>
@@ -6554,7 +7875,7 @@
         <v>36</v>
       </c>
       <c r="D28" t="s">
-        <v>42</v>
+        <v>90</v>
       </c>
       <c r="E28" t="s">
         <v>37</v>
@@ -6605,12 +7926,12 @@
         <v>24</v>
       </c>
       <c r="U28" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B29">
         <v>200664076</v>
@@ -6628,7 +7949,7 @@
         <v>34</v>
       </c>
       <c r="G29" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="H29" t="s">
         <v>24</v>
@@ -6675,7 +7996,7 @@
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B30">
         <v>201122222</v>
@@ -6684,7 +8005,7 @@
         <v>36</v>
       </c>
       <c r="D30" t="s">
-        <v>42</v>
+        <v>91</v>
       </c>
       <c r="E30" t="s">
         <v>37</v>
@@ -6735,21 +8056,21 @@
         <v>23</v>
       </c>
       <c r="U30" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B31">
         <v>201358229</v>
       </c>
       <c r="C31" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="D31" t="s">
-        <v>42</v>
+        <v>90</v>
       </c>
       <c r="E31" t="s">
         <v>37</v>
@@ -6805,7 +8126,7 @@
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B32">
         <v>201328739</v>
@@ -6814,13 +8135,13 @@
         <v>36</v>
       </c>
       <c r="D32" t="s">
-        <v>42</v>
+        <v>90</v>
       </c>
       <c r="E32" t="s">
         <v>33</v>
       </c>
       <c r="F32" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G32" t="s">
         <v>29</v>
@@ -6865,12 +8186,12 @@
         <v>24</v>
       </c>
       <c r="U32" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="B33">
         <v>201504145</v>
@@ -6885,7 +8206,7 @@
         <v>33</v>
       </c>
       <c r="F33" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G33" t="s">
         <v>22</v>
@@ -6935,16 +8256,16 @@
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="B34">
         <v>201303453</v>
       </c>
       <c r="C34" t="s">
-        <v>84</v>
+        <v>31</v>
       </c>
       <c r="D34" t="s">
-        <v>42</v>
+        <v>90</v>
       </c>
       <c r="E34" t="s">
         <v>37</v>
@@ -7000,25 +8321,25 @@
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="B35">
         <v>201337092</v>
       </c>
       <c r="C35" t="s">
-        <v>74</v>
+        <v>36</v>
       </c>
       <c r="D35" t="s">
-        <v>42</v>
+        <v>90</v>
       </c>
       <c r="E35" t="s">
         <v>37</v>
       </c>
       <c r="F35" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G35" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="H35" t="s">
         <v>24</v>
@@ -7065,16 +8386,16 @@
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="B36">
         <v>20134865</v>
       </c>
       <c r="C36" t="s">
-        <v>84</v>
+        <v>31</v>
       </c>
       <c r="D36" t="s">
-        <v>42</v>
+        <v>90</v>
       </c>
       <c r="E36" t="s">
         <v>33</v>
@@ -7130,7 +8451,7 @@
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="B37">
         <v>20131526</v>
@@ -7139,16 +8460,16 @@
         <v>36</v>
       </c>
       <c r="D37" t="s">
-        <v>42</v>
+        <v>90</v>
       </c>
       <c r="E37" t="s">
         <v>37</v>
       </c>
       <c r="F37" t="s">
-        <v>88</v>
+        <v>38</v>
       </c>
       <c r="G37" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="H37" t="s">
         <v>23</v>
@@ -7195,16 +8516,16 @@
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="B38">
         <v>201314912</v>
       </c>
       <c r="C38" t="s">
-        <v>74</v>
+        <v>36</v>
       </c>
       <c r="D38" t="s">
-        <v>42</v>
+        <v>90</v>
       </c>
       <c r="E38" t="s">
         <v>33</v>
@@ -7213,7 +8534,7 @@
         <v>28</v>
       </c>
       <c r="G38" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="H38" t="s">
         <v>23</v>
@@ -7266,10 +8587,10 @@
         <v>201689078</v>
       </c>
       <c r="C39" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="D39" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="E39" t="s">
         <v>33</v>
@@ -7331,7 +8652,7 @@
         <v>201489146</v>
       </c>
       <c r="C40" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="D40" t="s">
         <v>40</v>
@@ -7396,10 +8717,10 @@
         <v>201152036</v>
       </c>
       <c r="C41" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D41" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="E41" t="s">
         <v>33</v>
@@ -7461,7 +8782,7 @@
         <v>201406760</v>
       </c>
       <c r="C42" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D42" t="s">
         <v>40</v>
@@ -7526,7 +8847,7 @@
         <v>201510694</v>
       </c>
       <c r="C43" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="D43" t="s">
         <v>32</v>
@@ -7591,7 +8912,7 @@
         <v>201502985</v>
       </c>
       <c r="C44" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="D44" t="s">
         <v>32</v>
@@ -7603,7 +8924,7 @@
         <v>34</v>
       </c>
       <c r="G44" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="H44" t="s">
         <v>23</v>
@@ -7840,7 +9161,7 @@
         <v>23</v>
       </c>
       <c r="U47" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="49" spans="4:20" x14ac:dyDescent="0.25">
@@ -7977,6 +9298,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -7984,8 +9306,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:B25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8000,7 +9322,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -8048,10 +9370,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:B9"/>
+  <dimension ref="A3:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8065,12 +9387,12 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B4" s="3">
         <v>12</v>
@@ -8086,34 +9408,191 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B6" s="3">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="3">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:C16"/>
+  <sheetViews>
+    <sheetView topLeftCell="C4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N16" sqref="N16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.88671875" customWidth="1"/>
+    <col min="3" max="3" width="20.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
         <v>88</v>
       </c>
-      <c r="B7" s="3">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C4" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C7" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>38</v>
-      </c>
-      <c r="B8" s="3">
+        <v>40</v>
+      </c>
+      <c r="B8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="3">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>34</v>
-      </c>
-      <c r="B9" s="3">
-        <v>22</v>
+        <v>40</v>
+      </c>
+      <c r="B9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C9" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" t="s">
+        <v>93</v>
+      </c>
+      <c r="C10" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>86</v>
+      </c>
+      <c r="B11" t="s">
+        <v>92</v>
+      </c>
+      <c r="C11" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>89</v>
+      </c>
+      <c r="B12" t="s">
+        <v>89</v>
+      </c>
+      <c r="C12" s="3"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>90</v>
+      </c>
+      <c r="B13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>90</v>
+      </c>
+      <c r="B14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>90</v>
+      </c>
+      <c r="B15" t="s">
+        <v>93</v>
+      </c>
+      <c r="C15" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>91</v>
+      </c>
+      <c r="B16" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="3">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Corrected year level based on student no.
</commit_message>
<xml_diff>
--- a/results_charted.xlsx
+++ b/results_charted.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="Raw Data" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="31" r:id="rId5"/>
+    <pivotCache cacheId="0" r:id="rId5"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -313,7 +313,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -444,6 +444,12 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Fira Mono"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Fira Mono"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -798,7 +804,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -977,7 +983,6 @@
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
-          <c:layout/>
           <c:spPr>
             <a:solidFill>
               <a:sysClr val="window" lastClr="FFFFFF"/>
@@ -1032,7 +1037,6 @@
                   <a:noFill/>
                 </a:ln>
               </c15:spPr>
-              <c15:layout/>
             </c:ext>
           </c:extLst>
         </c:dLbl>
@@ -1148,6 +1152,50 @@
             </c:ext>
           </c:extLst>
         </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="6"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+          <a:scene3d>
+            <a:camera prst="orthographicFront"/>
+            <a:lightRig rig="brightRoom" dir="t"/>
+          </a:scene3d>
+          <a:sp3d prstMaterial="flat">
+            <a:bevelT w="50800" h="101600" prst="angle"/>
+            <a:contourClr>
+              <a:srgbClr val="000000"/>
+            </a:contourClr>
+          </a:sp3d>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="7"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+          <a:scene3d>
+            <a:camera prst="orthographicFront"/>
+            <a:lightRig rig="brightRoom" dir="t"/>
+          </a:scene3d>
+          <a:sp3d prstMaterial="flat">
+            <a:bevelT w="50800" h="101600" prst="angle"/>
+            <a:contourClr>
+              <a:srgbClr val="000000"/>
+            </a:contourClr>
+          </a:sp3d>
+        </c:spPr>
       </c:pivotFmt>
     </c:pivotFmts>
     <c:plotArea>
@@ -1905,6 +1953,49 @@
     <c:pivotFmts>
       <c:pivotFmt>
         <c:idx val="0"/>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="1"/>
+        <c:spPr>
+          <a:gradFill rotWithShape="1">
+            <a:gsLst>
+              <a:gs pos="0">
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="110000"/>
+                  <a:satMod val="105000"/>
+                  <a:tint val="67000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="50000">
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="105000"/>
+                  <a:satMod val="103000"/>
+                  <a:tint val="73000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="100000">
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="105000"/>
+                  <a:satMod val="109000"/>
+                  <a:tint val="81000"/>
+                </a:schemeClr>
+              </a:gs>
+            </a:gsLst>
+            <a:lin ang="5400000" scaled="0"/>
+          </a:gradFill>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:shade val="95000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
       </c:pivotFmt>
     </c:pivotFmts>
     <c:plotArea>
@@ -5236,7 +5327,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable21" cacheId="31" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable21" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="1">
   <location ref="A3:B5" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="21">
     <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
@@ -5408,12 +5499,36 @@
   <dataFields count="1">
     <dataField name="Count of Sex" fld="4" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
-  <chartFormats count="1">
+  <chartFormats count="3">
     <chartFormat chart="0" format="5" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
             <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="6">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="4" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="7">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="4" count="1" selected="0">
+            <x v="1"/>
           </reference>
         </references>
       </pivotArea>
@@ -5429,7 +5544,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable28" cacheId="31" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable28" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="1">
   <location ref="A3:B7" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="21">
     <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
@@ -5632,7 +5747,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="31" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="2">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="2">
   <location ref="A3:C16" firstHeaderRow="1" firstDataRow="1" firstDataCol="2"/>
   <pivotFields count="21">
     <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
@@ -5869,7 +5984,7 @@
     <dataField name="Count of Year Level" fld="3" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
   <chartFormats count="1">
-    <chartFormat chart="0" format="2" series="1">
+    <chartFormat chart="0" format="1" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -6093,8 +6208,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V52"/>
   <sheetViews>
-    <sheetView topLeftCell="C28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F52" sqref="F52"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7745,7 +7860,7 @@
         <v>36</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>91</v>
+        <v>32</v>
       </c>
       <c r="E26" t="s">
         <v>37</v>
@@ -9306,7 +9421,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:B25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
@@ -9433,7 +9548,7 @@
   <dimension ref="A3:C16"/>
   <sheetViews>
     <sheetView topLeftCell="C4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Removed non-Engg and non-CS respondents
</commit_message>
<xml_diff>
--- a/results_charted.xlsx
+++ b/results_charted.xlsx
@@ -19,13 +19,13 @@
   </sheets>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId5"/>
+    <pivotCache cacheId="30" r:id="rId5"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="975" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="830" uniqueCount="87">
   <si>
     <t>Timestamp</t>
   </si>
@@ -246,9 +246,6 @@
     <t>2016/09/19 9:37:35 PM GMT+8</t>
   </si>
   <si>
-    <t>2016/09/19 11:38:42 PM GMT+8</t>
-  </si>
-  <si>
     <t>2016/09/20 12:03:39 AM GMT+8</t>
   </si>
   <si>
@@ -276,21 +273,6 @@
     <t>Count of Sex</t>
   </si>
   <si>
-    <t>College of Fine Arts</t>
-  </si>
-  <si>
-    <t>1st Year</t>
-  </si>
-  <si>
-    <t>College of Human Kinetics</t>
-  </si>
-  <si>
-    <t>6th Year</t>
-  </si>
-  <si>
-    <t>Virata School of Business</t>
-  </si>
-  <si>
     <t>Count of Year Level</t>
   </si>
   <si>
@@ -303,10 +285,7 @@
     <t>5th Year</t>
   </si>
   <si>
-    <t>College of Arts and Letters</t>
-  </si>
-  <si>
-    <t>College of Social Science and Philosophy</t>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -1349,10 +1328,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>26</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1685,7 +1664,7 @@
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>22</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2058,70 +2037,46 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>'Year Level'!$A$4:$B$16</c:f>
+              <c:f>'Year Level'!$A$4:$B$10</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="13"/>
+                <c:ptCount val="7"/>
                 <c:lvl>
                   <c:pt idx="0">
-                    <c:v>College of Fine Arts</c:v>
+                    <c:v>College of Engineering</c:v>
                   </c:pt>
                   <c:pt idx="1">
+                    <c:v>College of Science</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
                     <c:v>College of Engineering</c:v>
                   </c:pt>
-                  <c:pt idx="2">
-                    <c:v>College of Science</c:v>
-                  </c:pt>
                   <c:pt idx="3">
-                    <c:v>Virata School of Business</c:v>
+                    <c:v>(blank)</c:v>
                   </c:pt>
                   <c:pt idx="4">
                     <c:v>College of Engineering</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>College of Human Kinetics</c:v>
+                    <c:v>College of Science</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>College of Social Science and Philosophy</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>College of Arts and Letters</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>(blank)</c:v>
-                  </c:pt>
-                  <c:pt idx="9">
-                    <c:v>College of Engineering</c:v>
-                  </c:pt>
-                  <c:pt idx="10">
-                    <c:v>College of Science</c:v>
-                  </c:pt>
-                  <c:pt idx="11">
-                    <c:v>College of Social Science and Philosophy</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
                     <c:v>College of Engineering</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
-                    <c:v>1st Year</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
                     <c:v>2nd Year</c:v>
                   </c:pt>
-                  <c:pt idx="4">
+                  <c:pt idx="2">
                     <c:v>3rd Year</c:v>
                   </c:pt>
-                  <c:pt idx="7">
-                    <c:v>6th Year</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
+                  <c:pt idx="3">
                     <c:v>(blank)</c:v>
                   </c:pt>
-                  <c:pt idx="9">
+                  <c:pt idx="4">
                     <c:v>4th Year</c:v>
                   </c:pt>
-                  <c:pt idx="12">
+                  <c:pt idx="6">
                     <c:v>5th Year</c:v>
                   </c:pt>
                 </c:lvl>
@@ -2130,45 +2085,27 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Year Level'!$C$4:$C$16</c:f>
+              <c:f>'Year Level'!$C$4:$C$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>2</c:v>
+                <c:pt idx="4">
+                  <c:v>15</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>1</c:v>
-                </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>9</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4151,34 +4088,34 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Vincent Paul Fiestada" refreshedDate="42634.876256828706" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="46">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Vincent Paul Fiestada" refreshedDate="42634.886243171299" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="39">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A1:U47" sheet="Raw Data"/>
+    <worksheetSource ref="A1:U40" sheet="Raw Data"/>
   </cacheSource>
   <cacheFields count="21">
     <cacheField name="Timestamp" numFmtId="0">
       <sharedItems containsDate="1" containsMixedTypes="1" minDate="2016-09-20T00:00:00" maxDate="2016-09-21T00:00:00"/>
     </cacheField>
     <cacheField name="Student Number" numFmtId="0">
-      <sharedItems containsMixedTypes="1" containsNumber="1" containsInteger="1" minValue="20131526" maxValue="201689078"/>
+      <sharedItems containsMixedTypes="1" containsNumber="1" containsInteger="1" minValue="20131526" maxValue="201523456"/>
     </cacheField>
     <cacheField name="College" numFmtId="0">
       <sharedItems containsBlank="1" count="15">
         <m/>
         <s v="College of Engineering"/>
         <s v="College of Science"/>
-        <s v="College of Social Science and Philosophy"/>
-        <s v="College of Fine Arts"/>
-        <s v="College of Human Kinetics"/>
-        <s v="College of Arts and Letters"/>
-        <s v="Virata School of Business"/>
         <s v="(CSSP)College of Social Sciences &amp; Philosophy" u="1"/>
         <s v="CSSP" u="1"/>
+        <s v="College of Arts and Letters" u="1"/>
         <s v=" College of Engineering" u="1"/>
         <s v="Engineering" u="1"/>
+        <s v="College of Social Science and Philosophy" u="1"/>
+        <s v="Virata School of Business" u="1"/>
+        <s v="College of Fine Arts" u="1"/>
         <s v="CS" u="1"/>
         <s v="(CAL)College of Arts &amp; Letters" u="1"/>
         <s v="ENGG" u="1"/>
+        <s v="College of Human Kinetics" u="1"/>
       </sharedItems>
     </cacheField>
     <cacheField name="Year Level" numFmtId="0">
@@ -4188,9 +4125,9 @@
         <s v="2nd Year"/>
         <s v="3rd Year"/>
         <s v="5th Year"/>
-        <s v="1st Year"/>
-        <s v="6th Year"/>
+        <s v="6th Year" u="1"/>
         <s v="4th - 5th Year" u="1"/>
+        <s v="1st Year" u="1"/>
       </sharedItems>
     </cacheField>
     <cacheField name="Sex" numFmtId="0">
@@ -4264,7 +4201,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="46">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="39">
   <r>
     <s v="2016/09/13 10:50:44 PM GMT+8"/>
     <s v="Carina Tesoro"/>
@@ -4821,7 +4758,7 @@
     <s v="2016/09/19 8:09:26 PM GMT+8"/>
     <n v="201523456"/>
     <x v="1"/>
-    <x v="4"/>
+    <x v="2"/>
     <x v="1"/>
     <x v="1"/>
     <s v="iPhones &amp; iPads;Galaxy Phones &amp; Tablets;Java;Android"/>
@@ -4933,29 +4870,6 @@
     <s v="None of their profits"/>
   </r>
   <r>
-    <s v="2016/09/19 11:38:42 PM GMT+8"/>
-    <n v="201358229"/>
-    <x v="3"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="1"/>
-    <s v="iPhones &amp; iPads;Galaxy Phones &amp; Tablets;Java;Android"/>
-    <s v="Yes"/>
-    <s v="Yes"/>
-    <s v="No"/>
-    <s v="Yes"/>
-    <s v="Yes"/>
-    <s v="No"/>
-    <s v="Yes"/>
-    <s v="Yes"/>
-    <s v="No"/>
-    <s v="Yes"/>
-    <s v="Yes"/>
-    <s v="No"/>
-    <s v="No"/>
-    <s v="Just a part of their profits"/>
-  </r>
-  <r>
     <s v="2016/09/20 12:03:39 AM GMT+8"/>
     <n v="201328739"/>
     <x v="1"/>
@@ -5118,144 +5032,6 @@
   </r>
   <r>
     <d v="2016-09-20T00:00:00"/>
-    <n v="201689078"/>
-    <x v="4"/>
-    <x v="5"/>
-    <x v="0"/>
-    <x v="1"/>
-    <s v="iPhones &amp; iPads;Galaxy Phones &amp; Tablets;Android"/>
-    <s v="No"/>
-    <s v="Yes"/>
-    <s v="Yes"/>
-    <s v="No"/>
-    <s v="No"/>
-    <s v="No"/>
-    <s v="No"/>
-    <s v="No"/>
-    <s v="Yes"/>
-    <s v="Yes"/>
-    <s v="No"/>
-    <s v="Yes"/>
-    <s v="Yes"/>
-    <s v="Just a part of their profits"/>
-  </r>
-  <r>
-    <d v="2016-09-20T00:00:00"/>
-    <n v="201489146"/>
-    <x v="5"/>
-    <x v="3"/>
-    <x v="1"/>
-    <x v="1"/>
-    <s v="iPhones &amp; iPads;Galaxy Phones &amp; Tablets;Android"/>
-    <s v="Yes"/>
-    <s v="Yes"/>
-    <s v="Yes"/>
-    <s v="Yes"/>
-    <s v="Yes"/>
-    <s v="Yes"/>
-    <s v="No"/>
-    <s v="Yes"/>
-    <s v="No"/>
-    <s v="Yes"/>
-    <s v="Yes"/>
-    <s v="No"/>
-    <s v="No"/>
-    <s v="Just a part of their profits"/>
-  </r>
-  <r>
-    <d v="2016-09-20T00:00:00"/>
-    <n v="201152036"/>
-    <x v="6"/>
-    <x v="6"/>
-    <x v="0"/>
-    <x v="1"/>
-    <s v="iPhones &amp; iPads;Galaxy Phones &amp; Tablets;Java;Android"/>
-    <s v="No"/>
-    <s v="Yes"/>
-    <s v="Yes"/>
-    <s v="No"/>
-    <s v="Yes"/>
-    <s v="Yes"/>
-    <s v="No"/>
-    <s v="Yes"/>
-    <s v="No"/>
-    <s v="Yes"/>
-    <s v="No"/>
-    <s v="Yes"/>
-    <s v="Yes"/>
-    <s v="Just a part of their profits"/>
-  </r>
-  <r>
-    <d v="2016-09-20T00:00:00"/>
-    <n v="201406760"/>
-    <x v="3"/>
-    <x v="3"/>
-    <x v="0"/>
-    <x v="1"/>
-    <s v="iPhones &amp; iPads;Galaxy Phones &amp; Tablets;Java;Android"/>
-    <s v="Yes"/>
-    <s v="No"/>
-    <s v="No"/>
-    <s v="Yes"/>
-    <s v="Yes"/>
-    <s v="No"/>
-    <s v="No"/>
-    <s v="No"/>
-    <s v="No"/>
-    <s v="Yes"/>
-    <s v="Yes"/>
-    <s v="No"/>
-    <s v="Yes"/>
-    <s v="Just a part of their profits"/>
-  </r>
-  <r>
-    <d v="2016-09-20T00:00:00"/>
-    <n v="201510694"/>
-    <x v="7"/>
-    <x v="2"/>
-    <x v="0"/>
-    <x v="1"/>
-    <s v="iPhones &amp; iPads;Galaxy Phones &amp; Tablets;Android"/>
-    <s v="No"/>
-    <s v="No"/>
-    <s v="No"/>
-    <s v="Yes"/>
-    <s v="No"/>
-    <s v="Yes"/>
-    <s v="No"/>
-    <s v="Yes"/>
-    <s v="Yes"/>
-    <s v="Yes"/>
-    <s v="No"/>
-    <s v="No"/>
-    <s v="Yes"/>
-    <s v="Just a part of their profits"/>
-  </r>
-  <r>
-    <d v="2016-09-20T00:00:00"/>
-    <n v="201502985"/>
-    <x v="7"/>
-    <x v="2"/>
-    <x v="0"/>
-    <x v="1"/>
-    <s v="Android"/>
-    <s v="No"/>
-    <s v="No"/>
-    <s v="No"/>
-    <s v="Yes"/>
-    <s v="Yes"/>
-    <s v="No"/>
-    <s v="No"/>
-    <s v="No"/>
-    <s v="Yes"/>
-    <s v="Yes"/>
-    <s v="No"/>
-    <s v="No"/>
-    <s v="No"/>
-    <s v="Just a part of their profits"/>
-  </r>
-  <r>
-    <d v="2016-09-20T00:00:00"/>
     <n v="201504580"/>
     <x v="1"/>
     <x v="2"/>
@@ -5327,7 +5103,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable21" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable21" cacheId="30" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="1">
   <location ref="A3:B5" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="21">
     <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
@@ -5544,7 +5320,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable28" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable28" cacheId="30" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="1">
   <location ref="A3:B7" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="21">
     <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
@@ -5747,8 +5523,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="2">
-  <location ref="A3:C16" firstHeaderRow="1" firstDataRow="1" firstDataCol="2"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="30" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="2">
+  <location ref="A3:C10" firstHeaderRow="1" firstDataRow="1" firstDataCol="2"/>
   <pivotFields count="21">
     <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
       <extLst>
@@ -5766,21 +5542,21 @@
     </pivotField>
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
       <items count="15">
+        <item m="1" x="6"/>
+        <item m="1" x="12"/>
+        <item m="1" x="3"/>
+        <item x="1"/>
         <item m="1" x="10"/>
+        <item m="1" x="14"/>
+        <item x="2"/>
+        <item m="1" x="11"/>
+        <item m="1" x="4"/>
         <item m="1" x="13"/>
+        <item m="1" x="7"/>
+        <item m="1" x="9"/>
+        <item x="0"/>
         <item m="1" x="8"/>
-        <item x="1"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="2"/>
-        <item m="1" x="12"/>
-        <item m="1" x="9"/>
-        <item m="1" x="14"/>
-        <item m="1" x="11"/>
-        <item x="7"/>
-        <item x="0"/>
-        <item x="3"/>
-        <item x="6"/>
+        <item m="1" x="5"/>
       </items>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
@@ -5790,11 +5566,11 @@
     </pivotField>
     <pivotField axis="axisRow" dataField="1" compact="0" outline="0" showAll="0" defaultSubtotal="0">
       <items count="8">
-        <item x="5"/>
+        <item m="1" x="7"/>
         <item x="2"/>
         <item x="3"/>
-        <item m="1" x="7"/>
-        <item x="6"/>
+        <item m="1" x="6"/>
+        <item m="1" x="5"/>
         <item x="0"/>
         <item x="1"/>
         <item x="4"/>
@@ -5929,11 +5705,7 @@
     <field x="3"/>
     <field x="2"/>
   </rowFields>
-  <rowItems count="13">
-    <i>
-      <x/>
-      <x v="4"/>
-    </i>
+  <rowItems count="7">
     <i>
       <x v="1"/>
       <x v="3"/>
@@ -5941,22 +5713,9 @@
     <i r="1">
       <x v="6"/>
     </i>
-    <i r="1">
-      <x v="11"/>
-    </i>
     <i>
       <x v="2"/>
       <x v="3"/>
-    </i>
-    <i r="1">
-      <x v="5"/>
-    </i>
-    <i r="1">
-      <x v="13"/>
-    </i>
-    <i>
-      <x v="4"/>
-      <x v="14"/>
     </i>
     <i>
       <x v="5"/>
@@ -5968,9 +5727,6 @@
     </i>
     <i r="1">
       <x v="6"/>
-    </i>
-    <i r="1">
-      <x v="13"/>
     </i>
     <i>
       <x v="7"/>
@@ -6206,10 +5962,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V52"/>
+  <dimension ref="A1:V46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="B28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6362,7 +6118,7 @@
         <v>36</v>
       </c>
       <c r="D3" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="E3" t="s">
         <v>33</v>
@@ -6625,7 +6381,7 @@
         <v>31</v>
       </c>
       <c r="D7" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="E7" t="s">
         <v>33</v>
@@ -6755,7 +6511,7 @@
         <v>31</v>
       </c>
       <c r="D9" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="E9" t="s">
         <v>33</v>
@@ -6820,7 +6576,7 @@
         <v>36</v>
       </c>
       <c r="D10" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="E10" t="s">
         <v>37</v>
@@ -6950,7 +6706,7 @@
         <v>36</v>
       </c>
       <c r="D12" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="E12" t="s">
         <v>37</v>
@@ -7015,7 +6771,7 @@
         <v>36</v>
       </c>
       <c r="D13" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="E13" t="s">
         <v>33</v>
@@ -7080,7 +6836,7 @@
         <v>36</v>
       </c>
       <c r="D14" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="E14" t="s">
         <v>33</v>
@@ -7145,7 +6901,7 @@
         <v>36</v>
       </c>
       <c r="D15" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="E15" t="s">
         <v>37</v>
@@ -7210,7 +6966,7 @@
         <v>36</v>
       </c>
       <c r="D16" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="E16" t="s">
         <v>33</v>
@@ -7275,7 +7031,7 @@
         <v>36</v>
       </c>
       <c r="D17" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="E17" t="s">
         <v>33</v>
@@ -7340,7 +7096,7 @@
         <v>36</v>
       </c>
       <c r="D18" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="E18" t="s">
         <v>37</v>
@@ -7405,7 +7161,7 @@
         <v>36</v>
       </c>
       <c r="D19" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="E19" t="s">
         <v>37</v>
@@ -7470,7 +7226,7 @@
         <v>36</v>
       </c>
       <c r="D20" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="E20" t="s">
         <v>33</v>
@@ -7535,7 +7291,7 @@
         <v>36</v>
       </c>
       <c r="D21" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="E21" t="s">
         <v>37</v>
@@ -7600,7 +7356,7 @@
         <v>36</v>
       </c>
       <c r="D22" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="E22" t="s">
         <v>37</v>
@@ -7665,7 +7421,7 @@
         <v>36</v>
       </c>
       <c r="D23" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="E23" t="s">
         <v>37</v>
@@ -7730,7 +7486,7 @@
         <v>36</v>
       </c>
       <c r="D24" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="E24" t="s">
         <v>33</v>
@@ -7795,7 +7551,7 @@
         <v>36</v>
       </c>
       <c r="D25" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="E25" t="s">
         <v>33</v>
@@ -7925,7 +7681,7 @@
         <v>36</v>
       </c>
       <c r="D27" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="E27" t="s">
         <v>37</v>
@@ -7990,7 +7746,7 @@
         <v>36</v>
       </c>
       <c r="D28" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="E28" t="s">
         <v>37</v>
@@ -8120,7 +7876,7 @@
         <v>36</v>
       </c>
       <c r="D30" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="E30" t="s">
         <v>37</v>
@@ -8179,64 +7935,64 @@
         <v>73</v>
       </c>
       <c r="B31">
-        <v>201358229</v>
+        <v>201328739</v>
       </c>
       <c r="C31" t="s">
-        <v>93</v>
+        <v>36</v>
       </c>
       <c r="D31" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="E31" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F31" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="G31" t="s">
         <v>29</v>
       </c>
       <c r="H31" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I31" t="s">
         <v>24</v>
       </c>
       <c r="J31" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="K31" t="s">
         <v>24</v>
       </c>
       <c r="L31" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M31" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="N31" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="O31" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="P31" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="Q31" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R31" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S31" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="T31" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="U31" t="s">
-        <v>25</v>
+        <v>52</v>
       </c>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.25">
@@ -8244,13 +8000,13 @@
         <v>74</v>
       </c>
       <c r="B32">
-        <v>201328739</v>
+        <v>201504145</v>
       </c>
       <c r="C32" t="s">
         <v>36</v>
       </c>
       <c r="D32" t="s">
-        <v>90</v>
+        <v>32</v>
       </c>
       <c r="E32" t="s">
         <v>33</v>
@@ -8259,22 +8015,22 @@
         <v>46</v>
       </c>
       <c r="G32" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="H32" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I32" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J32" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K32" t="s">
         <v>24</v>
       </c>
       <c r="L32" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="M32" t="s">
         <v>24</v>
@@ -8301,7 +8057,7 @@
         <v>24</v>
       </c>
       <c r="U32" t="s">
-        <v>52</v>
+        <v>25</v>
       </c>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.25">
@@ -8309,34 +8065,34 @@
         <v>75</v>
       </c>
       <c r="B33">
-        <v>201504145</v>
+        <v>201303453</v>
       </c>
       <c r="C33" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D33" t="s">
-        <v>32</v>
+        <v>84</v>
       </c>
       <c r="E33" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="F33" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="G33" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="H33" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I33" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J33" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="K33" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L33" t="s">
         <v>24</v>
@@ -8363,7 +8119,7 @@
         <v>24</v>
       </c>
       <c r="T33" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="U33" t="s">
         <v>25</v>
@@ -8374,25 +8130,25 @@
         <v>76</v>
       </c>
       <c r="B34">
-        <v>201303453</v>
+        <v>201337092</v>
       </c>
       <c r="C34" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="D34" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="E34" t="s">
         <v>37</v>
       </c>
       <c r="F34" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="G34" t="s">
-        <v>29</v>
+        <v>60</v>
       </c>
       <c r="H34" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I34" t="s">
         <v>24</v>
@@ -8401,13 +8157,13 @@
         <v>24</v>
       </c>
       <c r="K34" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L34" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M34" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N34" t="s">
         <v>23</v>
@@ -8419,13 +8175,13 @@
         <v>24</v>
       </c>
       <c r="Q34" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="R34" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="S34" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="T34" t="s">
         <v>23</v>
@@ -8439,25 +8195,25 @@
         <v>77</v>
       </c>
       <c r="B35">
-        <v>201337092</v>
+        <v>20134865</v>
       </c>
       <c r="C35" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D35" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="E35" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F35" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="G35" t="s">
-        <v>60</v>
+        <v>22</v>
       </c>
       <c r="H35" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I35" t="s">
         <v>24</v>
@@ -8469,19 +8225,19 @@
         <v>24</v>
       </c>
       <c r="L35" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="M35" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="N35" t="s">
         <v>23</v>
       </c>
       <c r="O35" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="P35" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q35" t="s">
         <v>24</v>
@@ -8504,22 +8260,22 @@
         <v>78</v>
       </c>
       <c r="B36">
-        <v>20134865</v>
+        <v>20131526</v>
       </c>
       <c r="C36" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="D36" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="E36" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="F36" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="G36" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="H36" t="s">
         <v>23</v>
@@ -8528,10 +8284,10 @@
         <v>24</v>
       </c>
       <c r="J36" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K36" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L36" t="s">
         <v>24</v>
@@ -8543,19 +8299,19 @@
         <v>23</v>
       </c>
       <c r="O36" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="P36" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="Q36" t="s">
         <v>24</v>
       </c>
       <c r="R36" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S36" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="T36" t="s">
         <v>23</v>
@@ -8569,19 +8325,19 @@
         <v>79</v>
       </c>
       <c r="B37">
-        <v>20131526</v>
+        <v>201314912</v>
       </c>
       <c r="C37" t="s">
         <v>36</v>
       </c>
       <c r="D37" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="E37" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F37" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="G37" t="s">
         <v>50</v>
@@ -8596,7 +8352,7 @@
         <v>23</v>
       </c>
       <c r="K37" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L37" t="s">
         <v>24</v>
@@ -8608,19 +8364,19 @@
         <v>23</v>
       </c>
       <c r="O37" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="P37" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q37" t="s">
         <v>24</v>
       </c>
       <c r="R37" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="S37" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="T37" t="s">
         <v>23</v>
@@ -8630,26 +8386,26 @@
       </c>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>80</v>
+      <c r="A38" s="1">
+        <v>42633</v>
       </c>
       <c r="B38">
-        <v>201314912</v>
+        <v>201504580</v>
       </c>
       <c r="C38" t="s">
         <v>36</v>
       </c>
       <c r="D38" t="s">
-        <v>90</v>
+        <v>32</v>
       </c>
       <c r="E38" t="s">
         <v>33</v>
       </c>
       <c r="F38" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="G38" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="H38" t="s">
         <v>23</v>
@@ -8688,7 +8444,7 @@
         <v>23</v>
       </c>
       <c r="T38" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="U38" t="s">
         <v>25</v>
@@ -8699,13 +8455,13 @@
         <v>42633</v>
       </c>
       <c r="B39">
-        <v>201689078</v>
+        <v>201504560</v>
       </c>
       <c r="C39" t="s">
-        <v>83</v>
+        <v>36</v>
       </c>
       <c r="D39" t="s">
-        <v>84</v>
+        <v>32</v>
       </c>
       <c r="E39" t="s">
         <v>33</v>
@@ -8714,7 +8470,7 @@
         <v>34</v>
       </c>
       <c r="G39" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="H39" t="s">
         <v>23</v>
@@ -8723,37 +8479,37 @@
         <v>24</v>
       </c>
       <c r="J39" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K39" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L39" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="M39" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="N39" t="s">
         <v>23</v>
       </c>
       <c r="O39" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="P39" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q39" t="s">
         <v>24</v>
       </c>
       <c r="R39" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="S39" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="T39" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="U39" t="s">
         <v>25</v>
@@ -8764,13 +8520,13 @@
         <v>42633</v>
       </c>
       <c r="B40">
-        <v>201489146</v>
+        <v>201502082</v>
       </c>
       <c r="C40" t="s">
-        <v>85</v>
+        <v>31</v>
       </c>
       <c r="D40" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="E40" t="s">
         <v>37</v>
@@ -8779,22 +8535,22 @@
         <v>34</v>
       </c>
       <c r="G40" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="H40" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I40" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J40" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K40" t="s">
         <v>24</v>
       </c>
       <c r="L40" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M40" t="s">
         <v>24</v>
@@ -8803,10 +8559,10 @@
         <v>23</v>
       </c>
       <c r="O40" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="P40" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="Q40" t="s">
         <v>24</v>
@@ -8821,594 +8577,148 @@
         <v>23</v>
       </c>
       <c r="U40" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A41" s="1">
-        <v>42633</v>
-      </c>
-      <c r="B41">
-        <v>201152036</v>
-      </c>
-      <c r="C41" t="s">
-        <v>92</v>
-      </c>
-      <c r="D41" t="s">
-        <v>86</v>
-      </c>
-      <c r="E41" t="s">
-        <v>33</v>
-      </c>
-      <c r="F41" t="s">
-        <v>34</v>
-      </c>
-      <c r="G41" t="s">
-        <v>29</v>
-      </c>
-      <c r="H41" t="s">
-        <v>23</v>
-      </c>
-      <c r="I41" t="s">
-        <v>24</v>
-      </c>
-      <c r="J41" t="s">
-        <v>24</v>
-      </c>
-      <c r="K41" t="s">
-        <v>23</v>
-      </c>
-      <c r="L41" t="s">
-        <v>24</v>
-      </c>
-      <c r="M41" t="s">
-        <v>24</v>
-      </c>
-      <c r="N41" t="s">
-        <v>23</v>
-      </c>
-      <c r="O41" t="s">
-        <v>24</v>
-      </c>
-      <c r="P41" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q41" t="s">
-        <v>24</v>
-      </c>
-      <c r="R41" t="s">
-        <v>23</v>
-      </c>
-      <c r="S41" t="s">
-        <v>24</v>
-      </c>
-      <c r="T41" t="s">
-        <v>24</v>
-      </c>
-      <c r="U41" t="s">
-        <v>25</v>
+        <v>52</v>
       </c>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A42" s="1">
-        <v>42633</v>
-      </c>
-      <c r="B42">
-        <v>201406760</v>
-      </c>
-      <c r="C42" t="s">
-        <v>93</v>
-      </c>
       <c r="D42" t="s">
-        <v>40</v>
-      </c>
-      <c r="E42" t="s">
-        <v>33</v>
-      </c>
-      <c r="F42" t="s">
-        <v>34</v>
-      </c>
-      <c r="G42" t="s">
+        <v>24</v>
+      </c>
+      <c r="H42">
+        <f>COUNTIF(H2:H40, "Yes")</f>
+        <v>18</v>
+      </c>
+      <c r="I42">
+        <f>COUNTIF(I2:I40, "Yes")</f>
+        <v>13</v>
+      </c>
+      <c r="J42">
+        <f>COUNTIF(J2:J40, "Yes")</f>
+        <v>16</v>
+      </c>
+      <c r="K42">
+        <f>COUNTIF(K2:K40, "Yes")</f>
+        <v>31</v>
+      </c>
+      <c r="L42">
+        <f>COUNTIF(L2:L40, "Yes")</f>
+        <v>32</v>
+      </c>
+      <c r="M42">
+        <f>COUNTIF(M2:M40, "Yes")</f>
+        <v>26</v>
+      </c>
+      <c r="N42">
+        <f>COUNTIF(N2:N40, "Yes")</f>
+        <v>4</v>
+      </c>
+      <c r="O42">
+        <f>COUNTIF(O2:O40, "Yes")</f>
+        <v>19</v>
+      </c>
+      <c r="P42">
+        <f>COUNTIF(P2:P40, "Yes")</f>
+        <v>22</v>
+      </c>
+      <c r="Q42">
+        <f>COUNTIF(Q2:Q40, "Yes")</f>
         <v>29</v>
       </c>
-      <c r="H42" t="s">
-        <v>24</v>
-      </c>
-      <c r="I42" t="s">
-        <v>23</v>
-      </c>
-      <c r="J42" t="s">
-        <v>23</v>
-      </c>
-      <c r="K42" t="s">
-        <v>24</v>
-      </c>
-      <c r="L42" t="s">
-        <v>24</v>
-      </c>
-      <c r="M42" t="s">
-        <v>23</v>
-      </c>
-      <c r="N42" t="s">
-        <v>23</v>
-      </c>
-      <c r="O42" t="s">
-        <v>23</v>
-      </c>
-      <c r="P42" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q42" t="s">
-        <v>24</v>
-      </c>
-      <c r="R42" t="s">
-        <v>24</v>
-      </c>
-      <c r="S42" t="s">
-        <v>23</v>
-      </c>
-      <c r="T42" t="s">
-        <v>24</v>
-      </c>
-      <c r="U42" t="s">
+      <c r="R42">
+        <f>COUNTIF(R2:R40, "Yes")</f>
         <v>25</v>
+      </c>
+      <c r="S42">
+        <f>COUNTIF(S2:S40, "Yes")</f>
+        <v>19</v>
+      </c>
+      <c r="T42">
+        <f>COUNTIF(T2:T40, "Yes")</f>
+        <v>19</v>
       </c>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A43" s="1">
-        <v>42633</v>
-      </c>
-      <c r="B43">
-        <v>201510694</v>
-      </c>
-      <c r="C43" t="s">
-        <v>87</v>
-      </c>
       <c r="D43" t="s">
-        <v>32</v>
-      </c>
-      <c r="E43" t="s">
-        <v>33</v>
-      </c>
-      <c r="F43" t="s">
-        <v>34</v>
-      </c>
-      <c r="G43" t="s">
-        <v>22</v>
-      </c>
-      <c r="H43" t="s">
-        <v>23</v>
-      </c>
-      <c r="I43" t="s">
-        <v>23</v>
-      </c>
-      <c r="J43" t="s">
-        <v>23</v>
-      </c>
-      <c r="K43" t="s">
-        <v>24</v>
-      </c>
-      <c r="L43" t="s">
-        <v>23</v>
-      </c>
-      <c r="M43" t="s">
-        <v>24</v>
-      </c>
-      <c r="N43" t="s">
-        <v>23</v>
-      </c>
-      <c r="O43" t="s">
-        <v>24</v>
-      </c>
-      <c r="P43" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q43" t="s">
-        <v>24</v>
-      </c>
-      <c r="R43" t="s">
-        <v>23</v>
-      </c>
-      <c r="S43" t="s">
-        <v>23</v>
-      </c>
-      <c r="T43" t="s">
-        <v>24</v>
-      </c>
-      <c r="U43" t="s">
-        <v>25</v>
+        <v>23</v>
+      </c>
+      <c r="H43">
+        <f>COUNTIF(H2:H40, "No")</f>
+        <v>21</v>
+      </c>
+      <c r="I43">
+        <f t="shared" ref="I43:T43" si="0">COUNTIF(I2:I40, "No")</f>
+        <v>26</v>
+      </c>
+      <c r="J43">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="K43">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="L43">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="M43">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="N43">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="O43">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="P43">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="Q43">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="R43">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="S43">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="T43">
+        <f t="shared" si="0"/>
+        <v>20</v>
       </c>
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A44" s="1">
-        <v>42633</v>
-      </c>
-      <c r="B44">
-        <v>201502985</v>
-      </c>
-      <c r="C44" t="s">
-        <v>87</v>
-      </c>
       <c r="D44" t="s">
-        <v>32</v>
-      </c>
-      <c r="E44" t="s">
-        <v>33</v>
-      </c>
-      <c r="F44" t="s">
-        <v>34</v>
-      </c>
-      <c r="G44" t="s">
-        <v>50</v>
-      </c>
-      <c r="H44" t="s">
-        <v>23</v>
-      </c>
-      <c r="I44" t="s">
-        <v>23</v>
-      </c>
-      <c r="J44" t="s">
-        <v>23</v>
-      </c>
-      <c r="K44" t="s">
-        <v>24</v>
-      </c>
-      <c r="L44" t="s">
-        <v>24</v>
-      </c>
-      <c r="M44" t="s">
-        <v>23</v>
-      </c>
-      <c r="N44" t="s">
-        <v>23</v>
-      </c>
-      <c r="O44" t="s">
-        <v>23</v>
-      </c>
-      <c r="P44" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q44" t="s">
-        <v>24</v>
-      </c>
-      <c r="R44" t="s">
-        <v>23</v>
-      </c>
-      <c r="S44" t="s">
-        <v>23</v>
-      </c>
-      <c r="T44" t="s">
-        <v>23</v>
-      </c>
-      <c r="U44" t="s">
-        <v>25</v>
+        <v>37</v>
+      </c>
+      <c r="E44">
+        <f>COUNTIF(E2:E40, "Male")</f>
+        <v>18</v>
       </c>
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A45" s="1">
-        <v>42633</v>
-      </c>
-      <c r="B45">
-        <v>201504580</v>
-      </c>
-      <c r="C45" t="s">
-        <v>36</v>
-      </c>
       <c r="D45" t="s">
-        <v>32</v>
-      </c>
-      <c r="E45" t="s">
         <v>33</v>
       </c>
-      <c r="F45" t="s">
-        <v>34</v>
-      </c>
-      <c r="G45" t="s">
-        <v>29</v>
-      </c>
-      <c r="H45" t="s">
-        <v>23</v>
-      </c>
-      <c r="I45" t="s">
-        <v>24</v>
-      </c>
-      <c r="J45" t="s">
-        <v>23</v>
-      </c>
-      <c r="K45" t="s">
-        <v>24</v>
-      </c>
-      <c r="L45" t="s">
-        <v>24</v>
-      </c>
-      <c r="M45" t="s">
-        <v>24</v>
-      </c>
-      <c r="N45" t="s">
-        <v>23</v>
-      </c>
-      <c r="O45" t="s">
-        <v>24</v>
-      </c>
-      <c r="P45" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q45" t="s">
-        <v>24</v>
-      </c>
-      <c r="R45" t="s">
-        <v>24</v>
-      </c>
-      <c r="S45" t="s">
-        <v>23</v>
-      </c>
-      <c r="T45" t="s">
-        <v>24</v>
-      </c>
-      <c r="U45" t="s">
-        <v>25</v>
+      <c r="E45">
+        <f>COUNTIF(E2:E40, "Female")</f>
+        <v>21</v>
       </c>
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A46" s="1">
-        <v>42633</v>
-      </c>
-      <c r="B46">
-        <v>201504560</v>
-      </c>
-      <c r="C46" t="s">
-        <v>36</v>
-      </c>
       <c r="D46" t="s">
-        <v>32</v>
-      </c>
-      <c r="E46" t="s">
-        <v>33</v>
-      </c>
-      <c r="F46" t="s">
-        <v>34</v>
-      </c>
-      <c r="G46" t="s">
-        <v>29</v>
-      </c>
-      <c r="H46" t="s">
-        <v>23</v>
-      </c>
-      <c r="I46" t="s">
-        <v>24</v>
-      </c>
-      <c r="J46" t="s">
-        <v>23</v>
-      </c>
-      <c r="K46" t="s">
-        <v>24</v>
-      </c>
-      <c r="L46" t="s">
-        <v>24</v>
-      </c>
-      <c r="M46" t="s">
-        <v>24</v>
-      </c>
-      <c r="N46" t="s">
-        <v>23</v>
-      </c>
-      <c r="O46" t="s">
-        <v>24</v>
-      </c>
-      <c r="P46" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q46" t="s">
-        <v>24</v>
-      </c>
-      <c r="R46" t="s">
-        <v>24</v>
-      </c>
-      <c r="S46" t="s">
-        <v>23</v>
-      </c>
-      <c r="T46" t="s">
-        <v>23</v>
-      </c>
-      <c r="U46" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A47" s="1">
-        <v>42633</v>
-      </c>
-      <c r="B47">
-        <v>201502082</v>
-      </c>
-      <c r="C47" t="s">
-        <v>31</v>
-      </c>
-      <c r="D47" t="s">
-        <v>32</v>
-      </c>
-      <c r="E47" t="s">
-        <v>37</v>
-      </c>
-      <c r="F47" t="s">
-        <v>34</v>
-      </c>
-      <c r="G47" t="s">
-        <v>29</v>
-      </c>
-      <c r="H47" t="s">
-        <v>23</v>
-      </c>
-      <c r="I47" t="s">
-        <v>23</v>
-      </c>
-      <c r="J47" t="s">
-        <v>23</v>
-      </c>
-      <c r="K47" t="s">
-        <v>24</v>
-      </c>
-      <c r="L47" t="s">
-        <v>23</v>
-      </c>
-      <c r="M47" t="s">
-        <v>24</v>
-      </c>
-      <c r="N47" t="s">
-        <v>23</v>
-      </c>
-      <c r="O47" t="s">
-        <v>23</v>
-      </c>
-      <c r="P47" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q47" t="s">
-        <v>24</v>
-      </c>
-      <c r="R47" t="s">
-        <v>24</v>
-      </c>
-      <c r="S47" t="s">
-        <v>23</v>
-      </c>
-      <c r="T47" t="s">
-        <v>23</v>
-      </c>
-      <c r="U47" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="49" spans="4:20" x14ac:dyDescent="0.25">
-      <c r="D49" t="s">
-        <v>24</v>
-      </c>
-      <c r="H49">
-        <f>COUNTIF(H2:H47, "Yes")</f>
-        <v>21</v>
-      </c>
-      <c r="I49">
-        <f t="shared" ref="I49:T49" si="0">COUNTIF(I2:I47, "Yes")</f>
-        <v>17</v>
-      </c>
-      <c r="J49">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-      <c r="K49">
-        <f t="shared" si="0"/>
-        <v>36</v>
-      </c>
-      <c r="L49">
-        <f t="shared" si="0"/>
-        <v>37</v>
-      </c>
-      <c r="M49">
-        <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
-      <c r="N49">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="O49">
-        <f t="shared" si="0"/>
-        <v>23</v>
-      </c>
-      <c r="P49">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="Q49">
-        <f t="shared" si="0"/>
-        <v>36</v>
-      </c>
-      <c r="R49">
-        <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-      <c r="S49">
-        <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-      <c r="T49">
-        <f t="shared" si="0"/>
-        <v>23</v>
-      </c>
-    </row>
-    <row r="50" spans="4:20" x14ac:dyDescent="0.25">
-      <c r="D50" t="s">
-        <v>23</v>
-      </c>
-      <c r="H50">
-        <f>COUNTIF(H2:H47, "No")</f>
-        <v>25</v>
-      </c>
-      <c r="I50">
-        <f t="shared" ref="I50:T50" si="1">COUNTIF(I2:I47, "No")</f>
-        <v>29</v>
-      </c>
-      <c r="J50">
-        <f t="shared" si="1"/>
-        <v>27</v>
-      </c>
-      <c r="K50">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="L50">
-        <f t="shared" si="1"/>
-        <v>9</v>
-      </c>
-      <c r="M50">
-        <f t="shared" si="1"/>
-        <v>17</v>
-      </c>
-      <c r="N50">
-        <f t="shared" si="1"/>
-        <v>41</v>
-      </c>
-      <c r="O50">
-        <f t="shared" si="1"/>
-        <v>23</v>
-      </c>
-      <c r="P50">
-        <f t="shared" si="1"/>
-        <v>21</v>
-      </c>
-      <c r="Q50">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="R50">
-        <f t="shared" si="1"/>
-        <v>18</v>
-      </c>
-      <c r="S50">
-        <f t="shared" si="1"/>
-        <v>25</v>
-      </c>
-      <c r="T50">
-        <f t="shared" si="1"/>
-        <v>23</v>
-      </c>
-    </row>
-    <row r="51" spans="4:20" x14ac:dyDescent="0.25">
-      <c r="D51" t="s">
-        <v>37</v>
-      </c>
-      <c r="E51">
-        <f>COUNTIF(E2:E47, "Male")</f>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="52" spans="4:20" x14ac:dyDescent="0.25">
-      <c r="D52" t="s">
-        <v>33</v>
-      </c>
-      <c r="E52">
-        <f>COUNTIF(E2:E47, "Female")</f>
-        <v>26</v>
+        <v>86</v>
+      </c>
+      <c r="E46">
+        <f>E44+E45</f>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -9422,7 +8732,7 @@
   <dimension ref="A3:B25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9437,7 +8747,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -9445,7 +8755,7 @@
         <v>33</v>
       </c>
       <c r="B4" s="3">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -9453,7 +8763,7 @@
         <v>37</v>
       </c>
       <c r="B5" s="3">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
@@ -9488,7 +8798,7 @@
   <dimension ref="A3:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9502,7 +8812,7 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -9534,7 +8844,7 @@
         <v>34</v>
       </c>
       <c r="B7" s="3">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -9545,16 +8855,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:C16"/>
+  <dimension ref="A3:C10"/>
   <sheetViews>
     <sheetView topLeftCell="C4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.88671875" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" customWidth="1"/>
     <col min="3" max="3" width="20.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -9566,18 +8876,18 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>84</v>
+        <v>32</v>
       </c>
       <c r="B4" t="s">
-        <v>83</v>
+        <v>36</v>
       </c>
       <c r="C4" s="3">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -9585,129 +8895,63 @@
         <v>32</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C5" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="C6" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>83</v>
       </c>
       <c r="B7" t="s">
-        <v>87</v>
-      </c>
-      <c r="C7" s="3">
-        <v>2</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="C7" s="3"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="B8" t="s">
         <v>36</v>
       </c>
       <c r="C8" s="3">
-        <v>4</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="B9" t="s">
-        <v>85</v>
+        <v>31</v>
       </c>
       <c r="C9" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>40</v>
+        <v>85</v>
       </c>
       <c r="B10" t="s">
-        <v>93</v>
+        <v>36</v>
       </c>
       <c r="C10" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>86</v>
-      </c>
-      <c r="B11" t="s">
-        <v>92</v>
-      </c>
-      <c r="C11" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>89</v>
-      </c>
-      <c r="B12" t="s">
-        <v>89</v>
-      </c>
-      <c r="C12" s="3"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>90</v>
-      </c>
-      <c r="B13" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" s="3">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>90</v>
-      </c>
-      <c r="B14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" s="3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>90</v>
-      </c>
-      <c r="B15" t="s">
-        <v>93</v>
-      </c>
-      <c r="C15" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>91</v>
-      </c>
-      <c r="B16" t="s">
-        <v>36</v>
-      </c>
-      <c r="C16" s="3">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>